<commit_message>
improve testcases + format
</commit_message>
<xml_diff>
--- a/tests/MockData/test_file.xlsx
+++ b/tests/MockData/test_file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">PKT</t>
   </si>
@@ -52,13 +52,25 @@
     <t xml:space="preserve"> Min Humidity</t>
   </si>
   <si>
+    <t xml:space="preserve">Events</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean VisibilityKm</t>
+  </si>
+  <si>
     <t xml:space="preserve">2004-07-01</t>
   </si>
   <si>
+    <t xml:space="preserve">Rain</t>
+  </si>
+  <si>
     <t xml:space="preserve">2004-07-02</t>
   </si>
   <si>
     <t xml:space="preserve">2004-07-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thunder</t>
   </si>
 </sst>
 </file>
@@ -160,15 +172,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -202,10 +216,16 @@
       <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>26</v>
@@ -233,11 +253,14 @@
       </c>
       <c r="J2" s="0" t="n">
         <v>39</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>23</v>
@@ -265,18 +288,18 @@
       </c>
       <c r="J3" s="0" t="n">
         <v>59</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>12.8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>19</v>
-      </c>
       <c r="D4" s="0" t="n">
         <v>19</v>
       </c>
@@ -297,6 +320,12 @@
       </c>
       <c r="J4" s="0" t="n">
         <v>49</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>11.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>